<commit_message>
colum selection fix for template
</commit_message>
<xml_diff>
--- a/WindowsFormsApplication1/results.xlsx
+++ b/WindowsFormsApplication1/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\privat\voltige\OxygeneIV\Vaulting\WindowsFormsApplication1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5FCC8E-EAF5-4B24-900A-36EF1969EAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AF2786-AA56-4B0E-9BC1-F2D638FE6758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-435" yWindow="195" windowWidth="29280" windowHeight="14385" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2268,7 +2268,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2279,7 +2279,8 @@
     <col min="5" max="5" width="6.75" style="11" customWidth="1"/>
     <col min="6" max="6" width="26.5" style="11" customWidth="1"/>
     <col min="7" max="12" width="10.625" style="11" customWidth="1"/>
-    <col min="13" max="14" width="10.625" style="11" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="2" style="11" customWidth="1"/>
+    <col min="14" max="14" width="2.375" style="11" customWidth="1"/>
     <col min="15" max="15" width="34.625" style="11" customWidth="1"/>
     <col min="16" max="109" width="10.625" style="11" customWidth="1"/>
     <col min="110" max="16384" width="10.625" style="11"/>
@@ -2441,7 +2442,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M7" s="50">
-        <f>IF(COUNTBLANK(H7:K7)=0,1,0)</f>
+        <f>IF(COUNTBLANK(H7:J7)=0,1,0)</f>
         <v>0</v>
       </c>
       <c r="N7" s="50">
@@ -2499,7 +2500,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M8" s="50">
-        <f>IF(COUNTBLANK(H8:K8)=0,1,0)</f>
+        <f t="shared" ref="M8:M10" si="0">IF(COUNTBLANK(H8:J8)=0,1,0)</f>
         <v>0</v>
       </c>
       <c r="N8" s="58">
@@ -2545,7 +2546,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M9" s="50">
-        <f>IF(COUNTBLANK(H9:K9)=0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" s="58">
@@ -2587,7 +2588,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M10" s="50">
-        <f>IF(COUNTBLANK(H10:K10)=0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" s="66">
@@ -2624,7 +2625,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="59" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;14
 </oddHeader>
@@ -4405,7 +4406,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView showRuler="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4577,7 +4578,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M7" s="192">
-        <f>IF(COUNTBLANK(H7:K7)=0,1,0)</f>
+        <f>IF(COUNTBLANK(H7:I7)=0,1,0)</f>
         <v>0</v>
       </c>
       <c r="N7" s="192">
@@ -4632,7 +4633,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M8" s="192">
-        <f>IF(COUNTBLANK(H8:K8)=0,1,0)</f>
+        <f t="shared" ref="M8:M10" si="0">IF(COUNTBLANK(H8:I8)=0,1,0)</f>
         <v>0</v>
       </c>
       <c r="N8" s="202">
@@ -4675,7 +4676,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M9" s="192">
-        <f>IF(COUNTBLANK(H9:K9)=0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" s="202">
@@ -4714,7 +4715,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M10" s="192">
-        <f>IF(COUNTBLANK(H10:K10)=0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" s="214">
@@ -5105,7 +5106,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView showRuler="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5116,7 +5117,7 @@
     <col min="5" max="5" width="6.75" style="11" customWidth="1"/>
     <col min="6" max="6" width="26.5" style="11" customWidth="1"/>
     <col min="7" max="12" width="10.625" style="11" customWidth="1"/>
-    <col min="13" max="14" width="10.625" style="11" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="2.5" style="11" customWidth="1"/>
     <col min="15" max="15" width="34.625" style="11" customWidth="1"/>
     <col min="16" max="109" width="10.625" style="11" customWidth="1"/>
     <col min="110" max="16384" width="10.625" style="11"/>
@@ -5278,7 +5279,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M7" s="50">
-        <f>IF(COUNTBLANK(H7:K7)=0,1,0)</f>
+        <f>IF(COUNTBLANK(H7:J7)=0,1,0)</f>
         <v>0</v>
       </c>
       <c r="N7" s="50">
@@ -5336,7 +5337,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M8" s="50">
-        <f>IF(COUNTBLANK(H8:K8)=0,1,0)</f>
+        <f t="shared" ref="M8:M10" si="0">IF(COUNTBLANK(H8:J8)=0,1,0)</f>
         <v>0</v>
       </c>
       <c r="N8" s="58">
@@ -5382,7 +5383,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M9" s="50">
-        <f>IF(COUNTBLANK(H9:K9)=0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" s="58">
@@ -5424,7 +5425,7 @@
         <v>-9.9999999999999995E-7</v>
       </c>
       <c r="M10" s="50">
-        <f>IF(COUNTBLANK(H10:K10)=0,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" s="66">
@@ -5466,7 +5467,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.11811023622047245"/>
-  <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;C&amp;14
 </oddHeader>

</xml_diff>

<commit_message>
prep for handover, fakedata + doc
</commit_message>
<xml_diff>
--- a/WindowsFormsApplication1/results.xlsx
+++ b/WindowsFormsApplication1/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\privat\voltige\OxygeneIV\Vaulting\WindowsFormsApplication1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4ADB019-6E6C-475B-AC6B-70EE8C244F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FD7484-F3C2-41FB-BCD1-CFD274708E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28005" yWindow="375" windowWidth="26085" windowHeight="13305" tabRatio="741" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2268,7 +2268,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4406,7 +4406,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView showRuler="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:R10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5106,7 +5106,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView showRuler="0" view="pageLayout" zoomScale="80" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:R10"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>